<commit_message>
create SubmitChangesService, allow to create change history, create reader and writer, create pdf generator
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">Yaroslav</t>
   </si>
   <si>
-    <t xml:space="preserve">Shkvarla</t>
+    <t xml:space="preserve">Shkvarlas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9929845</t>
   </si>
   <si>
     <t xml:space="preserve">slav.shkvarlo@gmail.com</t>
@@ -37,13 +40,19 @@
     <t xml:space="preserve">Petrenko</t>
   </si>
   <si>
+    <t xml:space="preserve">123456</t>
+  </si>
+  <si>
     <t xml:space="preserve">petro@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Ostap</t>
   </si>
   <si>
-    <t xml:space="preserve">Ostapenko</t>
+    <t xml:space="preserve">Ostapenkos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2223335</t>
   </si>
   <si>
     <t xml:space="preserve">ostap@gmail.com</t>
@@ -163,68 +172,77 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="12.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="12.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="12.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="n">
+      <c r="D1" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="D1" s="2" t="n">
-        <v>992984576</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
+      <c r="A2" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>123456789</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
+      <c r="A3" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="D3" s="2" t="n">
-        <v>222333456</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
complete registration and authorization, add checkstyle
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Shkvarla</t>
   </si>
   <si>
-    <t xml:space="preserve">992984</t>
+    <t xml:space="preserve">9929845</t>
   </si>
   <si>
     <t xml:space="preserve">slav.shkvarlo@gmail.com</t>
@@ -73,7 +73,7 @@
     <t xml:space="preserve">Slavenko</t>
   </si>
   <si>
-    <t xml:space="preserve">134566</t>
+    <t xml:space="preserve">1345666</t>
   </si>
   <si>
     <t xml:space="preserve">geroi@gmail.com</t>
@@ -225,7 +225,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>